<commit_message>
df and tibbles, indexes and the tibbles
the trouble with tibbles
</commit_message>
<xml_diff>
--- a/Ex_Files_Learning_R_Tidyverse/Exercise Files/04_02/data-raw/transit-data.xlsx
+++ b/Ex_Files_Learning_R_Tidyverse/Exercise Files/04_02/data-raw/transit-data.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinjhnhadley/Google Drive/VisibleData/Lynda-Courses/2017/Up-and-Running-with-the-tidyverse/Learning the R Tidyverse/Exercise Files/04_02/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinerovinski/Documents/GitHub/tutorialski_TidyverseLearning_-NOV2021_LinkedLearning-/Ex_Files_Learning_R_Tidyverse/Exercise Files/04_02/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A1C064-8E7E-1848-8A58-1D0FAE6AD49C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10240" yWindow="460" windowWidth="19200" windowHeight="21060" tabRatio="500"/>
+    <workbookView xWindow="6400" yWindow="460" windowWidth="19200" windowHeight="15540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
     <sheet name="transport data" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -1338,7 +1339,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1383,6 +1384,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1650,10 +1654,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -1728,11 +1732,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H672"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>